<commit_message>
Change the main sheet to be "Orders" and store the output files in App_Data folder
</commit_message>
<xml_diff>
--- a/JLPTProcessor/all-data-groupize.xlsx
+++ b/JLPTProcessor/all-data-groupize.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruaini/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE046418-1503-5241-849E-FD34F4E45D30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="29160" windowHeight="11720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendees" sheetId="1" r:id="rId1"/>
@@ -13,12 +19,12 @@
     <sheet name="Orders" sheetId="4" r:id="rId4"/>
     <sheet name="Flights" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="268">
   <si>
     <t>Event Report: Japanese Language Proficiency Test -July 2023</t>
   </si>
@@ -819,13 +825,16 @@
   </si>
   <si>
     <t>N2</t>
+  </si>
+  <si>
+    <t>Stripe Paid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -879,6 +888,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -925,7 +942,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -957,9 +974,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -991,6 +1026,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1166,37 +1219,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="52" width="25.7109375" customWidth="1"/>
+    <col min="1" max="52" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1234,7 +1287,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>136</v>
       </c>
@@ -1272,7 +1325,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -1310,7 +1363,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>150</v>
       </c>
@@ -1348,7 +1401,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -1386,7 +1439,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>160</v>
       </c>
@@ -1424,7 +1477,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>164</v>
       </c>
@@ -1468,37 +1521,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AN11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="52" width="25.7109375" customWidth="1"/>
+    <col min="1" max="52" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1620,7 +1673,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>136</v>
       </c>
@@ -1742,7 +1795,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -1864,7 +1917,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>160</v>
       </c>
@@ -1986,7 +2039,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -2108,7 +2161,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -2236,37 +2289,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AK12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="52" width="25.7109375" customWidth="1"/>
+    <col min="1" max="52" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -2379,7 +2432,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2393,7 +2446,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2407,7 +2460,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0</v>
       </c>
@@ -2421,7 +2474,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0</v>
       </c>
@@ -2435,7 +2488,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0</v>
       </c>
@@ -2449,7 +2502,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0</v>
       </c>
@@ -2469,37 +2522,39 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="52" width="25.7109375" customWidth="1"/>
+    <col min="1" max="52" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2528,7 +2583,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>136</v>
       </c>
@@ -2551,10 +2606,10 @@
         <v>262</v>
       </c>
       <c r="I7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -2577,10 +2632,10 @@
         <v>262</v>
       </c>
       <c r="I8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>150</v>
       </c>
@@ -2591,7 +2646,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -2614,10 +2669,10 @@
         <v>262</v>
       </c>
       <c r="I10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>160</v>
       </c>
@@ -2643,7 +2698,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>164</v>
       </c>
@@ -2666,7 +2721,7 @@
         <v>262</v>
       </c>
       <c r="I12" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -2675,37 +2730,37 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AX12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="52" width="25.7109375" customWidth="1"/>
+    <col min="1" max="52" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:50">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:50">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:50">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:50">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>89</v>
       </c>
@@ -2857,7 +2912,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:50">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2871,7 +2926,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:50">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2885,7 +2940,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:50">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0</v>
       </c>
@@ -2899,7 +2954,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:50">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0</v>
       </c>
@@ -2913,7 +2968,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:50">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0</v>
       </c>
@@ -2927,7 +2982,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:50">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0</v>
       </c>

</xml_diff>